<commit_message>
update data file for iter 8 (bootstrap)
</commit_message>
<xml_diff>
--- a/Test Cases/Iteration 8/Iteration 8 Test Cases.xlsx
+++ b/Test Cases/Iteration 8/Iteration 8 Test Cases.xlsx
@@ -9,11 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="4880" yWindow="1430" windowWidth="25520" windowHeight="15540" tabRatio="674" firstSheet="2" activeTab="3"/>
+    <workbookView xWindow="4880" yWindow="1430" windowWidth="25520" windowHeight="15540" tabRatio="674" firstSheet="1" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Client -  CRUD" sheetId="17" state="hidden" r:id="rId1"/>
-    <sheet name="8 - GenderNAge Report" sheetId="27" state="hidden" r:id="rId2"/>
+    <sheet name="8 - GenderNAge Report" sheetId="27" r:id="rId2"/>
     <sheet name="8 - Ranking" sheetId="26" r:id="rId3"/>
     <sheet name="8 - KPI" sheetId="25" r:id="rId4"/>
     <sheet name="7-Bootstrap" sheetId="22" r:id="rId5"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="457" uniqueCount="289">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="451" uniqueCount="289">
   <si>
     <t>No</t>
   </si>
@@ -1635,369 +1635,6 @@
 Jan 2014  - 0 Indo Visa :   0 Non-Indo Visa       
                   / No result
 Jan 2015 - 7 Indo Visa : 5 Non-Indo Visa
-Increase / Decrease - </t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Compare with Previous Month </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-Dec 2015 - 2 Indo Visa : 4 Non-Indo Visa
-Jan 2016 - 3 Indo Visa : 3 Non-Indo Visa
-Increase / Decrease -
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-Compare with Previous Year </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-Jan 2015  - 7 Indo Visa :   5 Non-Indo Visa
-Jan 2016 - 3 Indo Visa : 3 Non-Indo Visa
-Increase / Decrease - </t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Compare with Previous Month </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-May 2016 -  5 Indo Visa : 1 Non-Indo Visa
-June 2016 -  2 Indo Visa : 2 Non-Indo Visa
-Increase / Decrease - 
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-Compare with Previous Year </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-June 2015  -  7 Indo Visa :  4  Non-Indo Visa
-June 2016 -  2 Indo Visa : 2 Non-Indo Visa
-Increase / Decrease - </t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Compare with Previous Month </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-Dec 2014 -  0 Inpatient :  0 Outpatient
-                    / No result 
-Jan 2015 -   10 Inpatient :  19 Outpatient
-Increase / Decrease -
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-Compare with Previous Year </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-Jan 2014  -  0 Inpatient :  0 Outpatient       
-                  / No result
-Jan 2015 -  10 Inpatient : 19  Outpatient
-Increase / Decrease -</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Compare with Previous Month </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-Dec 2015 - 5 Inpatient : 27 Outpatient
-Jan 2016 -  7 Inpatient : 25 Outpatient
-Increase / Decrease - 
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-Compare with Previous Year </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-Jan 2015  - 10 Inpatient : 19  Outpatient
-Jan 2016 -  7 Inpatient : 25 Outpatient
-Increase / Decrease -</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Compare with Previous Month </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-May 2016 - 10 Inpatient : 26 Outpatient
-June 2016 - 5 Inpatient : 7 Outpatient
-Increase / Decrease - 
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Compare with Previous Year </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-June 2015  - 11 Inpatient : 13 Outpatient
-June 2016 -  5 Inpatient : 7 Outpatient
-Increase / Decrease -</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Compare with Previous Month</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> 
-Nov 2016 - 10 Inpatient : 14 Outpatient
-Dec 2016 - 8 Inpatient : 19 Outpatient
-Increase / Decrease -
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Compare with Previous Year </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-Dec 2015  -5 Inpatient : 27 Outpatient
-Dec 2016 - 8 Inpatient : 19 Outpatient
-Increase / Decrease - </t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Compare with Previous Month </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-Nov 2016 - 0 Indo Visa : 3 Non-Indo Visa
-Dec 2016 - 11 Indo Visa : 8 Non-Indo Visa
-Increase / Decrease -
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Compare with Previous Year </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-Dec 2015  - 2 Indo Visa :  4 Non-Indo Visa
-Dec 2016 - 11 Indo Visa : 8 Non-Indo Visa
 Increase / Decrease - </t>
     </r>
   </si>
@@ -2205,11 +1842,6 @@
     <t>0 - 10</t>
   </si>
   <si>
-    <t xml:space="preserve">                 Male : Female : Unknown
-Number  1
-%               1</t>
-  </si>
-  <si>
     <t>11 - 20</t>
   </si>
   <si>
@@ -2272,6 +1904,374 @@
     <t xml:space="preserve">                 Male : Female : Unknown
 Number   1
 %               9</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Compare with Previous Month </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Dec 2015 - 2 Indo Visa : 4 Non-Indo Visa
+Jan 2016 - 3 Indo Visa : 3 Non-Indo Visa
+Increase / Decrease :  50% Indo Visa : -25% non-indo visa
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Compare with Previous Year </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Jan 2015  - 7 Indo Visa :   5 Non-Indo Visa
+Jan 2016 - 3 Indo Visa : 3 Non-Indo Visa
+Increase / Decrease : -57% visa :  -40% non-visa</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Compare with Previous Month </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+May 2016 -  5 Indo Visa : 1 Non-Indo Visa
+June 2016 -  2 Indo Visa : 2 Non-Indo Visa
+Increase / Decrease : -60% indo : 100% non-indo
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Compare with Previous Year </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+June 2015  -  7 Indo Visa :  4  Non-Indo Visa
+June 2016 -  2 Indo Visa : 2 Non-Indo Visa
+Increase / Decrease : -72% : -50% </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Compare with Previous Month </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Nov 2016 - 0 Indo Visa : 3 Non-Indo Visa
+Dec 2016 - 11 Indo Visa : 8 Non-Indo Visa
+Increase / Decrease  - : 167% non-indo 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Compare with Previous Year </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Dec 2015  - 2 Indo Visa :  4 Non-Indo Visa
+Dec 2016 - 11 Indo Visa : 8 Non-Indo Visa
+Increase / Decrease: 450% : 100% </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Compare with Previous Month </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Dec 2014 -  0 Inpatient :  0 Outpatient
+                    / No result 
+Jan 2015 -   10 Inpatient :  19 Outpatient
+Increase / Decrease : -   
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Compare with Previous Year </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Jan 2014  -  0 Inpatient :  0 Outpatient       
+                  / No result
+Jan 2015 -  10 Inpatient : 19  Outpatient
+Increase / Decrease : - </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Compare with Previous Month </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Dec 2015 - 5 Inpatient : 27 Outpatient
+Jan 2016 -  7 Inpatient : 25 Outpatient
+Increase / Decrease 40%: -8%
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Compare with Previous Year </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Jan 2015  - 10 Inpatient : 19  Outpatient
+Jan 2016 -  7 Inpatient : 25 Outpatient
+Increase / Decrease : -30% : 32% </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Compare with Previous Month </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+May 2016 - 10 Inpatient : 26 Outpatient
+June 2016 - 5 Inpatient : 7 Outpatient
+Increase / Decrease : -50% : -73% 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Compare with Previous Year </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+June 2015  - 11 Inpatient : 13 Outpatient
+June 2016 -  5 Inpatient : 7 Outpatient
+Increase / Decrease : -54% : -46% </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Compare with Previous Month</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 
+Nov 2016 - 10 Inpatient : 14 Outpatient
+Dec 2016 - 8 Inpatient : 19 Outpatient
+Increase / Decrease  :   -20% :36% 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Compare with Previous Year </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Dec 2015  -5 Inpatient : 27 Outpatient
+Dec 2016 - 8 Inpatient : 19 Outpatient
+Increase / Decrease - 60% : -30%</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">                 Male : Female : Unknown
+Number  3        : 3             : 
+%               1</t>
   </si>
 </sst>
 </file>
@@ -2964,8 +2964,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -3011,10 +3011,10 @@
         <v>1</v>
       </c>
       <c r="B4" s="23" t="s">
-        <v>271</v>
+        <v>264</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>272</v>
+        <v>288</v>
       </c>
       <c r="D4" s="21"/>
       <c r="E4" s="21"/>
@@ -3022,10 +3022,10 @@
     <row r="5" spans="1:5" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A5" s="7"/>
       <c r="B5" s="23" t="s">
-        <v>273</v>
+        <v>265</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>274</v>
+        <v>266</v>
       </c>
       <c r="D5" s="21"/>
       <c r="E5" s="21"/>
@@ -3033,10 +3033,10 @@
     <row r="6" spans="1:5" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A6" s="7"/>
       <c r="B6" s="23" t="s">
-        <v>275</v>
+        <v>267</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>276</v>
+        <v>268</v>
       </c>
       <c r="D6" s="21"/>
       <c r="E6" s="21"/>
@@ -3044,10 +3044,10 @@
     <row r="7" spans="1:5" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A7" s="7"/>
       <c r="B7" s="23" t="s">
-        <v>277</v>
+        <v>269</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>278</v>
+        <v>270</v>
       </c>
       <c r="D7" s="21"/>
       <c r="E7" s="21"/>
@@ -3055,10 +3055,10 @@
     <row r="8" spans="1:5" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A8" s="7"/>
       <c r="B8" s="23" t="s">
-        <v>279</v>
+        <v>271</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>280</v>
+        <v>272</v>
       </c>
       <c r="D8" s="21"/>
       <c r="E8" s="21"/>
@@ -3066,10 +3066,10 @@
     <row r="9" spans="1:5" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A9" s="7"/>
       <c r="B9" s="23" t="s">
-        <v>281</v>
+        <v>273</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>282</v>
+        <v>274</v>
       </c>
       <c r="D9" s="21"/>
       <c r="E9" s="21"/>
@@ -3077,10 +3077,10 @@
     <row r="10" spans="1:5" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A10" s="7"/>
       <c r="B10" s="23" t="s">
-        <v>283</v>
+        <v>275</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>284</v>
+        <v>276</v>
       </c>
       <c r="D10" s="21"/>
       <c r="E10" s="21"/>
@@ -3088,10 +3088,10 @@
     <row r="11" spans="1:5" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A11" s="7"/>
       <c r="B11" s="23" t="s">
-        <v>285</v>
+        <v>277</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>286</v>
+        <v>278</v>
       </c>
       <c r="D11" s="21"/>
       <c r="E11" s="21"/>
@@ -3099,10 +3099,10 @@
     <row r="12" spans="1:5" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A12" s="7"/>
       <c r="B12" s="23" t="s">
-        <v>287</v>
+        <v>279</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>288</v>
+        <v>280</v>
       </c>
       <c r="D12" s="21"/>
       <c r="E12" s="21"/>
@@ -3116,8 +3116,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -3196,7 +3196,7 @@
         <v>239</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>264</v>
+        <v>257</v>
       </c>
       <c r="E5" s="5"/>
       <c r="F5" s="5"/>
@@ -3212,7 +3212,7 @@
         <v>240</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>265</v>
+        <v>258</v>
       </c>
       <c r="E6" s="5"/>
       <c r="F6" s="5"/>
@@ -3260,7 +3260,7 @@
         <v>247</v>
       </c>
       <c r="D9" s="16" t="s">
-        <v>266</v>
+        <v>259</v>
       </c>
       <c r="E9" s="5"/>
       <c r="F9" s="5"/>
@@ -3286,7 +3286,7 @@
         <v>8</v>
       </c>
       <c r="B11" s="15" t="s">
-        <v>267</v>
+        <v>260</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>250</v>
@@ -3302,7 +3302,7 @@
         <v>9</v>
       </c>
       <c r="B12" s="15" t="s">
-        <v>267</v>
+        <v>260</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>239</v>
@@ -3318,7 +3318,7 @@
         <v>10</v>
       </c>
       <c r="B13" s="15" t="s">
-        <v>267</v>
+        <v>260</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>240</v>
@@ -3459,8 +3459,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:F11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -3529,7 +3529,7 @@
         <v>229</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>257</v>
+        <v>281</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="139.5" x14ac:dyDescent="0.35">
@@ -3543,7 +3543,7 @@
         <v>230</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>258</v>
+        <v>282</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="139.5" x14ac:dyDescent="0.35">
@@ -3557,7 +3557,7 @@
         <v>231</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>263</v>
+        <v>283</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="170.5" x14ac:dyDescent="0.35">
@@ -3571,7 +3571,7 @@
         <v>233</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>259</v>
+        <v>284</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="139.5" x14ac:dyDescent="0.35">
@@ -3585,7 +3585,7 @@
         <v>234</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>260</v>
+        <v>285</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="139.5" x14ac:dyDescent="0.35">
@@ -3599,7 +3599,7 @@
         <v>235</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>261</v>
+        <v>286</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="139.5" x14ac:dyDescent="0.35">
@@ -3613,38 +3613,22 @@
         <v>236</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" ht="247" x14ac:dyDescent="0.35">
-      <c r="A12" s="2">
-        <v>9</v>
-      </c>
-      <c r="B12" s="15" t="s">
-        <v>267</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>239</v>
-      </c>
-      <c r="D12" s="16" t="s">
-        <v>252</v>
-      </c>
+        <v>287</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A12" s="2"/>
+      <c r="B12" s="15"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="16"/>
       <c r="E12" s="5"/>
       <c r="F12" s="5"/>
     </row>
-    <row r="13" spans="1:6" ht="354.5" x14ac:dyDescent="0.35">
-      <c r="A13" s="2">
-        <v>10</v>
-      </c>
-      <c r="B13" s="15" t="s">
-        <v>267</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>240</v>
-      </c>
-      <c r="D13" s="16" t="s">
-        <v>253</v>
-      </c>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A13" s="2"/>
+      <c r="B13" s="15"/>
+      <c r="C13" s="2"/>
+      <c r="D13" s="16"/>
       <c r="E13" s="5"/>
       <c r="F13" s="5"/>
     </row>
@@ -4168,13 +4152,13 @@
         <v>7</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>268</v>
+        <v>261</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>269</v>
+        <v>262</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>270</v>
+        <v>263</v>
       </c>
       <c r="E8" s="2"/>
     </row>

</xml_diff>

<commit_message>
Update data file + test case for Gender and age report
-
</commit_message>
<xml_diff>
--- a/Test Cases/Iteration 8/Iteration 8 Test Cases.xlsx
+++ b/Test Cases/Iteration 8/Iteration 8 Test Cases.xlsx
@@ -13,7 +13,7 @@
   </bookViews>
   <sheets>
     <sheet name="Client -  CRUD" sheetId="17" state="hidden" r:id="rId1"/>
-    <sheet name="8 - GenderNAge Report" sheetId="27" r:id="rId2"/>
+    <sheet name="9 - GenderNAge Report" sheetId="27" r:id="rId2"/>
     <sheet name="8 - Ranking" sheetId="26" r:id="rId3"/>
     <sheet name="8 - KPI" sheetId="25" r:id="rId4"/>
     <sheet name="7-Bootstrap" sheetId="22" r:id="rId5"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="451" uniqueCount="289">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="455" uniqueCount="294">
   <si>
     <t>No</t>
   </si>
@@ -1845,65 +1845,25 @@
     <t>11 - 20</t>
   </si>
   <si>
-    <t xml:space="preserve">                 Male : Female : Unknown
-Number  1
-%               2</t>
-  </si>
-  <si>
     <t>21 - 30</t>
   </si>
   <si>
-    <t xml:space="preserve">                 Male : Female : Unknown
-Number   1
-%               3</t>
-  </si>
-  <si>
     <t>31 - 40</t>
   </si>
   <si>
-    <t xml:space="preserve">                 Male : Female : Unknown
-Number   1
-%               4</t>
-  </si>
-  <si>
     <t>41 - 50</t>
   </si>
   <si>
-    <t xml:space="preserve">                 Male : Female : Unknown
-Number   1
-%               5</t>
-  </si>
-  <si>
     <t>51 - 60</t>
   </si>
   <si>
-    <t xml:space="preserve">                 Male : Female : Unknown
-Number   1
-%               6</t>
-  </si>
-  <si>
     <t>61 - 70</t>
   </si>
   <si>
-    <t xml:space="preserve">                 Male : Female : Unknown
-Number   1
-%               7</t>
-  </si>
-  <si>
     <t>71 - 80</t>
   </si>
   <si>
-    <t xml:space="preserve">                 Male : Female : Unknown
-Number   1
-%               8</t>
-  </si>
-  <si>
     <t xml:space="preserve">80 and above </t>
-  </si>
-  <si>
-    <t xml:space="preserve">                 Male : Female : Unknown
-Number   1
-%               9</t>
   </si>
   <si>
     <r>
@@ -2270,8 +2230,72 @@
   </si>
   <si>
     <t xml:space="preserve">                 Male : Female : Unknown
-Number  3        : 3             : 
-%               1</t>
+Number  3        :    3          :  32
+Gender% 50    :    50
+Overall%              </t>
+  </si>
+  <si>
+    <t xml:space="preserve">                 Male : Female : Unknown
+Number     3     :      4        : 25
+Gender %  43   :   57    
+Overall%           </t>
+  </si>
+  <si>
+    <t xml:space="preserve">                 Male : Female : Unknown
+Number   1      :        4      :       37
+Gender %  20  :  80    
+Overall%              </t>
+  </si>
+  <si>
+    <t xml:space="preserve">                 Male : Female : Unknown
+Number   14  :  13 : 95 
+Gender % 52 : 48      
+Overall%             </t>
+  </si>
+  <si>
+    <t xml:space="preserve">                 Male : Female : Unknown
+Number  11   : 8 : 97 
+Gender %  58 :   42  
+Overall%       </t>
+  </si>
+  <si>
+    <t xml:space="preserve">                 Male : Female : Unknown
+Number   18       :     5         : 83 
+Gender %      78 : 22
+Overall%              </t>
+  </si>
+  <si>
+    <t xml:space="preserve">                 Male : Female : Unknown
+Number   7  :   4   : 63
+Gender %     64 : 36  
+Overall%        </t>
+  </si>
+  <si>
+    <t xml:space="preserve">                 Male : Female : Unknown
+Number   4      :     2          :      28 
+Gender %   67 : 33    
+Overall%           </t>
+  </si>
+  <si>
+    <t xml:space="preserve">                 Male : Female : Unknown
+Number   0       :  2            : 5 
+Gender %   0 : 100   
+Overall%             </t>
+  </si>
+  <si>
+    <t xml:space="preserve">569 Clients with Age without Gender </t>
+  </si>
+  <si>
+    <t xml:space="preserve">106 Clients with Age and Gender </t>
+  </si>
+  <si>
+    <t xml:space="preserve">6 Female with no bd, 1 male with no bd, 100 clients without bd and gender </t>
+  </si>
+  <si>
+    <t xml:space="preserve">[NEED RECONFIRM] 668 Unique Clients </t>
+  </si>
+  <si>
+    <t>Current Iteration: 9</t>
   </si>
 </sst>
 </file>
@@ -2962,10 +2986,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E12"/>
+  <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -2977,7 +3001,7 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="19" t="s">
-        <v>226</v>
+        <v>293</v>
       </c>
       <c r="B1" s="22"/>
       <c r="C1" s="5"/>
@@ -2989,126 +3013,153 @@
       <c r="B2" s="22"/>
       <c r="C2" s="5"/>
     </row>
-    <row r="3" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A3" s="10" t="s">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A3" s="19" t="s">
+        <v>292</v>
+      </c>
+      <c r="B3" s="22"/>
+      <c r="C3" s="5"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A4" s="19" t="s">
+        <v>289</v>
+      </c>
+      <c r="B4" s="22"/>
+      <c r="C4" s="5"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A5" s="19" t="s">
+        <v>290</v>
+      </c>
+      <c r="B5" s="22"/>
+      <c r="C5" s="5"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A6" s="19" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="A7" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="20" t="s">
+      <c r="B7" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="11" t="s">
+      <c r="C7" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="11" t="s">
+      <c r="D7" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="E3" s="11" t="s">
+      <c r="E7" s="11" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="46.5" x14ac:dyDescent="0.35">
-      <c r="A4" s="7">
+    <row r="8" spans="1:5" ht="62" x14ac:dyDescent="0.35">
+      <c r="A8" s="7">
         <v>1</v>
       </c>
-      <c r="B4" s="23" t="s">
+      <c r="B8" s="23" t="s">
         <v>264</v>
       </c>
-      <c r="C4" s="7" t="s">
-        <v>288</v>
-      </c>
-      <c r="D4" s="21"/>
-      <c r="E4" s="21"/>
-    </row>
-    <row r="5" spans="1:5" ht="46.5" x14ac:dyDescent="0.35">
-      <c r="A5" s="7"/>
-      <c r="B5" s="23" t="s">
-        <v>265</v>
-      </c>
-      <c r="C5" s="7" t="s">
-        <v>266</v>
-      </c>
-      <c r="D5" s="21"/>
-      <c r="E5" s="21"/>
-    </row>
-    <row r="6" spans="1:5" ht="46.5" x14ac:dyDescent="0.35">
-      <c r="A6" s="7"/>
-      <c r="B6" s="23" t="s">
-        <v>267</v>
-      </c>
-      <c r="C6" s="7" t="s">
-        <v>268</v>
-      </c>
-      <c r="D6" s="21"/>
-      <c r="E6" s="21"/>
-    </row>
-    <row r="7" spans="1:5" ht="46.5" x14ac:dyDescent="0.35">
-      <c r="A7" s="7"/>
-      <c r="B7" s="23" t="s">
-        <v>269</v>
-      </c>
-      <c r="C7" s="7" t="s">
-        <v>270</v>
-      </c>
-      <c r="D7" s="21"/>
-      <c r="E7" s="21"/>
-    </row>
-    <row r="8" spans="1:5" ht="46.5" x14ac:dyDescent="0.35">
-      <c r="A8" s="7"/>
-      <c r="B8" s="23" t="s">
-        <v>271</v>
-      </c>
       <c r="C8" s="7" t="s">
-        <v>272</v>
+        <v>280</v>
       </c>
       <c r="D8" s="21"/>
       <c r="E8" s="21"/>
     </row>
-    <row r="9" spans="1:5" ht="46.5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" ht="62" x14ac:dyDescent="0.35">
       <c r="A9" s="7"/>
       <c r="B9" s="23" t="s">
-        <v>273</v>
+        <v>265</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>274</v>
+        <v>281</v>
       </c>
       <c r="D9" s="21"/>
       <c r="E9" s="21"/>
     </row>
-    <row r="10" spans="1:5" ht="46.5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:5" ht="62" x14ac:dyDescent="0.35">
       <c r="A10" s="7"/>
       <c r="B10" s="23" t="s">
-        <v>275</v>
+        <v>266</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>276</v>
+        <v>282</v>
       </c>
       <c r="D10" s="21"/>
       <c r="E10" s="21"/>
     </row>
-    <row r="11" spans="1:5" ht="46.5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:5" ht="62" x14ac:dyDescent="0.35">
       <c r="A11" s="7"/>
       <c r="B11" s="23" t="s">
-        <v>277</v>
+        <v>267</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>278</v>
+        <v>283</v>
       </c>
       <c r="D11" s="21"/>
       <c r="E11" s="21"/>
     </row>
-    <row r="12" spans="1:5" ht="46.5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:5" ht="62" x14ac:dyDescent="0.35">
       <c r="A12" s="7"/>
       <c r="B12" s="23" t="s">
-        <v>279</v>
+        <v>268</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>280</v>
+        <v>284</v>
       </c>
       <c r="D12" s="21"/>
       <c r="E12" s="21"/>
     </row>
+    <row r="13" spans="1:5" ht="62" x14ac:dyDescent="0.35">
+      <c r="A13" s="7"/>
+      <c r="B13" s="23" t="s">
+        <v>269</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>285</v>
+      </c>
+      <c r="D13" s="21"/>
+      <c r="E13" s="21"/>
+    </row>
+    <row r="14" spans="1:5" ht="62" x14ac:dyDescent="0.35">
+      <c r="A14" s="7"/>
+      <c r="B14" s="23" t="s">
+        <v>270</v>
+      </c>
+      <c r="C14" s="7" t="s">
+        <v>286</v>
+      </c>
+      <c r="D14" s="21"/>
+      <c r="E14" s="21"/>
+    </row>
+    <row r="15" spans="1:5" ht="62" x14ac:dyDescent="0.35">
+      <c r="A15" s="7"/>
+      <c r="B15" s="23" t="s">
+        <v>271</v>
+      </c>
+      <c r="C15" s="7" t="s">
+        <v>287</v>
+      </c>
+      <c r="D15" s="21"/>
+      <c r="E15" s="21"/>
+    </row>
+    <row r="16" spans="1:5" ht="62" x14ac:dyDescent="0.35">
+      <c r="A16" s="7"/>
+      <c r="B16" s="23" t="s">
+        <v>272</v>
+      </c>
+      <c r="C16" s="7" t="s">
+        <v>288</v>
+      </c>
+      <c r="D16" s="21"/>
+      <c r="E16" s="21"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -3529,7 +3580,7 @@
         <v>229</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>281</v>
+        <v>273</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="139.5" x14ac:dyDescent="0.35">
@@ -3543,7 +3594,7 @@
         <v>230</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>282</v>
+        <v>274</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="139.5" x14ac:dyDescent="0.35">
@@ -3557,7 +3608,7 @@
         <v>231</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>283</v>
+        <v>275</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="170.5" x14ac:dyDescent="0.35">
@@ -3571,7 +3622,7 @@
         <v>233</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>284</v>
+        <v>276</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="139.5" x14ac:dyDescent="0.35">
@@ -3585,7 +3636,7 @@
         <v>234</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>285</v>
+        <v>277</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="139.5" x14ac:dyDescent="0.35">
@@ -3599,7 +3650,7 @@
         <v>235</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>286</v>
+        <v>278</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="139.5" x14ac:dyDescent="0.35">
@@ -3613,7 +3664,7 @@
         <v>236</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>287</v>
+        <v>279</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.35">

</xml_diff>